<commit_message>
fixed delimiter in xls template
</commit_message>
<xml_diff>
--- a/Schablonen/Radiologie_ver1.41.xlsx
+++ b/Schablonen/Radiologie_ver1.41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5F2FF03-9808-43C7-BF5A-2B6AE0D12341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{746F5421-29A0-4FF9-A09C-AF76857A3C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -750,7 +750,7 @@
     <t>M1</t>
   </si>
   <si>
-    <t>nach …</t>
+    <t>nach ...</t>
   </si>
   <si>
     <t xml:space="preserve">Mediastinum [nach %M1%] verlagert. </t>
@@ -828,7 +828,7 @@
     <t>asc/desc</t>
   </si>
   <si>
-    <t>im Bereich der …</t>
+    <t>im Bereich der ...</t>
   </si>
   <si>
     <t>dilatiert bis %A3% mm im Bereich der %A2%.</t>
@@ -1745,8 +1745,8 @@
   <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="M107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P133" sqref="P133"/>
+      <pane ySplit="1" topLeftCell="K47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P71" sqref="P71"/>
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed unnecessary columns [Wenn] and [Baustein-ID] from xls template and Row Interface
</commit_message>
<xml_diff>
--- a/Schablonen/Radiologie_ver1.41.xlsx
+++ b/Schablonen/Radiologie_ver1.41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{746F5421-29A0-4FF9-A09C-AF76857A3C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42444FFE-F1F0-448B-B348-27E639E119F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="440">
   <si>
     <t>Typ</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Optional</t>
-  </si>
-  <si>
-    <t>Wenn</t>
-  </si>
-  <si>
-    <t>Baustein ID</t>
   </si>
   <si>
     <t>Baustein Befund</t>
@@ -1742,11 +1736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S132"/>
+  <dimension ref="A1:Q132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="K47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P71" sqref="P71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
@@ -1754,25 +1748,23 @@
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="72.5703125" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="41.28515625" customWidth="1"/>
-    <col min="14" max="14" width="35.7109375" customWidth="1"/>
-    <col min="15" max="15" width="40.5703125" customWidth="1"/>
-    <col min="16" max="16" width="39.140625" customWidth="1"/>
-    <col min="17" max="17" width="46.7109375" customWidth="1"/>
-    <col min="18" max="18" width="37.7109375" customWidth="1"/>
-    <col min="19" max="1026" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="72.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="41.28515625" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" customWidth="1"/>
+    <col min="13" max="13" width="40.5703125" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" customWidth="1"/>
+    <col min="15" max="15" width="46.7109375" customWidth="1"/>
+    <col min="16" max="16" width="37.7109375" customWidth="1"/>
+    <col min="17" max="1024" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1824,2151 +1816,2145 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:17">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:17">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="F4" t="s">
+    <row r="5" spans="1:17">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="O5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="6" spans="1:17">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>36</v>
       </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>37</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>38</v>
       </c>
-      <c r="P6" t="s">
+    </row>
+    <row r="7" spans="1:17">
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
+      <c r="O7" t="s">
         <v>42</v>
       </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="8" spans="1:17">
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="F8" t="s">
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="9" spans="1:17">
+      <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="E9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="F9" t="s">
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" t="s">
+    </row>
+    <row r="10" spans="1:17">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="M9" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
-      <c r="F10" t="s">
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="O11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
-      <c r="A11" t="s">
+    <row r="12" spans="1:17">
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="13" spans="1:17">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="F13" t="s">
+      <c r="J13" t="s">
         <v>60</v>
       </c>
-      <c r="G13" t="s">
+      <c r="K13" t="s">
         <v>61</v>
       </c>
       <c r="L13" t="s">
         <v>62</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>63</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>64</v>
       </c>
-      <c r="P13" t="s">
+    </row>
+    <row r="14" spans="1:17">
+      <c r="J14" t="s">
         <v>65</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="K14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
       <c r="L14" t="s">
         <v>67</v>
       </c>
-      <c r="M14" t="s">
+    </row>
+    <row r="15" spans="1:17">
+      <c r="J15" t="s">
         <v>68</v>
       </c>
-      <c r="N14" t="s">
+      <c r="K15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
       <c r="L15" t="s">
         <v>70</v>
       </c>
-      <c r="M15" t="s">
+    </row>
+    <row r="16" spans="1:17">
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="N15" t="s">
+      <c r="E16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="F16" t="s">
+      <c r="J16" t="s">
         <v>73</v>
       </c>
-      <c r="G16" t="s">
+      <c r="K16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" t="s">
         <v>74</v>
       </c>
-      <c r="L16" t="s">
+    </row>
+    <row r="17" spans="4:15">
+      <c r="J17" t="s">
         <v>75</v>
       </c>
-      <c r="M16" t="s">
+      <c r="K17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15">
+      <c r="J18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15">
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" t="s">
         <v>63</v>
       </c>
-      <c r="N16" t="s">
-        <v>64</v>
-      </c>
-      <c r="P16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="6:17">
-      <c r="L17" t="s">
-        <v>77</v>
-      </c>
-      <c r="M17" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="O19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15">
+      <c r="J20" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15">
+      <c r="J21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="6:17">
-      <c r="L18" t="s">
-        <v>78</v>
-      </c>
-      <c r="M18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="6:17">
-      <c r="F19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" t="s">
-        <v>81</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="L21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15">
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K22" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" t="s">
         <v>63</v>
       </c>
-      <c r="N19" t="s">
-        <v>64</v>
-      </c>
-      <c r="P19" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="6:17">
-      <c r="L20" t="s">
-        <v>83</v>
-      </c>
-      <c r="M20" t="s">
-        <v>68</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="O22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15">
+      <c r="J23" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15">
+      <c r="J24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="6:17">
-      <c r="L21" t="s">
-        <v>84</v>
-      </c>
-      <c r="M21" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="6:17">
-      <c r="F22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22" t="s">
-        <v>87</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="L24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" t="s">
         <v>63</v>
       </c>
-      <c r="N22" t="s">
-        <v>64</v>
-      </c>
-      <c r="P22" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="6:17">
-      <c r="L23" t="s">
-        <v>89</v>
-      </c>
-      <c r="M23" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="O25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15">
+      <c r="J26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="6:17">
-      <c r="L24" t="s">
-        <v>90</v>
-      </c>
-      <c r="M24" t="s">
-        <v>71</v>
-      </c>
-      <c r="N24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="6:17">
-      <c r="F25" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" t="s">
-        <v>91</v>
-      </c>
-      <c r="L25" t="s">
-        <v>92</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="L26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15">
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" t="s">
+        <v>95</v>
+      </c>
+      <c r="K27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" t="s">
         <v>63</v>
       </c>
-      <c r="N25" t="s">
-        <v>64</v>
-      </c>
-      <c r="P25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="6:17">
-      <c r="L26" t="s">
-        <v>94</v>
-      </c>
-      <c r="M26" t="s">
-        <v>71</v>
-      </c>
-      <c r="N26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="6:17">
-      <c r="F27" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="O27" t="s">
         <v>96</v>
       </c>
-      <c r="L27" t="s">
+    </row>
+    <row r="28" spans="4:15">
+      <c r="J28" t="s">
         <v>97</v>
       </c>
-      <c r="M27" t="s">
+      <c r="K28" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15">
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" t="s">
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" t="s">
         <v>63</v>
       </c>
-      <c r="N27" t="s">
-        <v>64</v>
-      </c>
-      <c r="P27" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="6:17">
-      <c r="L28" t="s">
-        <v>99</v>
-      </c>
-      <c r="M28" t="s">
-        <v>71</v>
-      </c>
-      <c r="N28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="6:17">
-      <c r="F29" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="O29" t="s">
         <v>101</v>
       </c>
-      <c r="L29" t="s">
+    </row>
+    <row r="30" spans="4:15">
+      <c r="J30" t="s">
         <v>102</v>
       </c>
-      <c r="M29" t="s">
+      <c r="K30" t="s">
+        <v>69</v>
+      </c>
+      <c r="L30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15">
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" t="s">
+        <v>61</v>
+      </c>
+      <c r="L31" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" t="s">
         <v>63</v>
       </c>
-      <c r="N29" t="s">
-        <v>64</v>
-      </c>
-      <c r="P29" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="6:17">
-      <c r="L30" t="s">
-        <v>104</v>
-      </c>
-      <c r="M30" t="s">
-        <v>71</v>
-      </c>
-      <c r="N30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="6:17">
-      <c r="F31" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="O31" t="s">
         <v>106</v>
       </c>
-      <c r="L31" t="s">
+    </row>
+    <row r="32" spans="4:15">
+      <c r="J32" t="s">
         <v>107</v>
       </c>
-      <c r="M31" t="s">
+      <c r="K32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15">
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="J33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="4:15">
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" t="s">
+        <v>112</v>
+      </c>
+      <c r="J34" t="s">
+        <v>113</v>
+      </c>
+      <c r="K34" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="4:15">
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>116</v>
+      </c>
+      <c r="J35" t="s">
+        <v>117</v>
+      </c>
+      <c r="K35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" t="s">
+        <v>70</v>
+      </c>
+      <c r="O35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="4:15">
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" t="s">
+        <v>120</v>
+      </c>
+      <c r="J36" t="s">
+        <v>121</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="4:15">
+      <c r="J37" t="s">
+        <v>123</v>
+      </c>
+      <c r="K37" t="s">
+        <v>124</v>
+      </c>
+      <c r="N37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="4:15">
+      <c r="D38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" t="s">
+        <v>127</v>
+      </c>
+      <c r="K38" t="s">
+        <v>61</v>
+      </c>
+      <c r="L38" t="s">
+        <v>62</v>
+      </c>
+      <c r="N38" t="s">
         <v>63</v>
       </c>
-      <c r="N31" t="s">
-        <v>64</v>
-      </c>
-      <c r="P31" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="6:17">
-      <c r="L32" t="s">
-        <v>109</v>
-      </c>
-      <c r="M32" t="s">
-        <v>71</v>
-      </c>
-      <c r="N32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="6:17">
-      <c r="F33" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" t="s">
-        <v>111</v>
-      </c>
-      <c r="L33" t="s">
-        <v>112</v>
-      </c>
-      <c r="M33" t="s">
-        <v>71</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="6:17">
-      <c r="F34" t="s">
-        <v>114</v>
-      </c>
-      <c r="G34" t="s">
-        <v>114</v>
-      </c>
-      <c r="L34" t="s">
-        <v>115</v>
-      </c>
-      <c r="M34" t="s">
-        <v>71</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="6:17">
-      <c r="F35" t="s">
-        <v>117</v>
-      </c>
-      <c r="G35" t="s">
-        <v>118</v>
-      </c>
-      <c r="L35" t="s">
-        <v>119</v>
-      </c>
-      <c r="M35" t="s">
-        <v>71</v>
-      </c>
-      <c r="N35" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="6:17">
-      <c r="F36" t="s">
-        <v>121</v>
-      </c>
-      <c r="G36" t="s">
-        <v>122</v>
-      </c>
-      <c r="L36" t="s">
-        <v>123</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="6:17">
-      <c r="L37" t="s">
-        <v>125</v>
-      </c>
-      <c r="M37" t="s">
-        <v>126</v>
-      </c>
-      <c r="P37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="6:17">
-      <c r="F38" t="s">
+      <c r="O38" t="s">
         <v>128</v>
       </c>
-      <c r="G38" t="s">
-        <v>128</v>
-      </c>
-      <c r="L38" t="s">
+    </row>
+    <row r="39" spans="4:15">
+      <c r="J39" t="s">
         <v>129</v>
       </c>
-      <c r="M38" t="s">
-        <v>63</v>
-      </c>
-      <c r="N38" t="s">
-        <v>64</v>
-      </c>
-      <c r="P38" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q38" t="s">
+      <c r="K39" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="39" spans="6:17">
       <c r="L39" t="s">
         <v>131</v>
       </c>
-      <c r="M39" t="s">
+    </row>
+    <row r="40" spans="4:15">
+      <c r="J40" t="s">
         <v>132</v>
       </c>
-      <c r="N39" t="s">
+      <c r="K40" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="40" spans="6:17">
       <c r="L40" t="s">
         <v>134</v>
       </c>
-      <c r="M40" t="s">
+    </row>
+    <row r="41" spans="4:15">
+      <c r="D41" t="s">
         <v>135</v>
       </c>
-      <c r="N40" t="s">
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="J41" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="41" spans="6:17">
-      <c r="F41" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="K41" t="s">
         <v>137</v>
       </c>
       <c r="L41" t="s">
         <v>138</v>
       </c>
-      <c r="M41" t="s">
+      <c r="O41" t="s">
         <v>139</v>
       </c>
-      <c r="N41" t="s">
+    </row>
+    <row r="42" spans="4:15">
+      <c r="J42" t="s">
         <v>140</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="K42" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="42" spans="6:17">
       <c r="L42" t="s">
         <v>142</v>
       </c>
-      <c r="M42" t="s">
+    </row>
+    <row r="43" spans="4:15">
+      <c r="F43" s="2"/>
+      <c r="J43" t="s">
         <v>143</v>
       </c>
-      <c r="N42" t="s">
+      <c r="K43" t="s">
+        <v>61</v>
+      </c>
+      <c r="L43" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="4:15">
+      <c r="F44" s="2"/>
+      <c r="J44" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="6:17">
-      <c r="H43" s="2"/>
-      <c r="L43" t="s">
+      <c r="K44" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="M43" t="s">
-        <v>63</v>
-      </c>
-      <c r="N43" t="s">
-        <v>64</v>
-      </c>
-      <c r="P43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="6:17">
-      <c r="H44" s="2"/>
       <c r="L44" t="s">
         <v>146</v>
       </c>
-      <c r="M44" s="3" t="s">
+      <c r="M44" s="4"/>
+      <c r="N44" t="s">
         <v>147</v>
       </c>
-      <c r="N44" t="s">
+    </row>
+    <row r="45" spans="4:15">
+      <c r="D45" t="s">
         <v>148</v>
       </c>
-      <c r="O44" s="4"/>
-      <c r="P44" t="s">
+      <c r="E45" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="45" spans="6:17">
-      <c r="F45" t="s">
+      <c r="J45" t="s">
         <v>150</v>
       </c>
-      <c r="G45" t="s">
+      <c r="K45" t="s">
         <v>151</v>
       </c>
       <c r="L45" t="s">
         <v>152</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>153</v>
       </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>154</v>
       </c>
-      <c r="P45" t="s">
+    </row>
+    <row r="46" spans="4:15">
+      <c r="D46" t="s">
         <v>155</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="E46" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="46" spans="6:17">
-      <c r="F46" t="s">
+      <c r="J46" t="s">
         <v>157</v>
       </c>
-      <c r="G46" t="s">
+      <c r="K46" t="s">
         <v>158</v>
       </c>
       <c r="L46" t="s">
         <v>159</v>
       </c>
-      <c r="M46" t="s">
+      <c r="O46" t="s">
         <v>160</v>
       </c>
-      <c r="N46" t="s">
+    </row>
+    <row r="47" spans="4:15">
+      <c r="D47" t="s">
         <v>161</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="E47" t="s">
+        <v>161</v>
+      </c>
+      <c r="J47" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="6:17">
-      <c r="F47" t="s">
+      <c r="K47" t="s">
+        <v>124</v>
+      </c>
+      <c r="N47" t="s">
         <v>163</v>
       </c>
-      <c r="G47" t="s">
-        <v>163</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="O47" t="s">
         <v>164</v>
       </c>
-      <c r="M47" t="s">
-        <v>126</v>
-      </c>
-      <c r="P47" t="s">
+    </row>
+    <row r="48" spans="4:15">
+      <c r="J48" t="s">
         <v>165</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="K48" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" spans="6:17">
       <c r="L48" t="s">
         <v>167</v>
       </c>
-      <c r="M48" t="s">
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="O49" t="s">
         <v>168</v>
       </c>
-      <c r="N48" t="s">
+    </row>
+    <row r="50" spans="1:17">
+      <c r="B50" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q49" t="s">
+      <c r="D50" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="B50" t="s">
+      <c r="E50" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="O50" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F50" t="s">
+      <c r="Q50" t="s">
         <v>172</v>
       </c>
-      <c r="G50" t="s">
-        <v>172</v>
-      </c>
-      <c r="H50" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q50" s="5" t="s">
+    </row>
+    <row r="51" spans="1:17">
+      <c r="D51" t="s">
         <v>173</v>
       </c>
-      <c r="S50" t="s">
+      <c r="E51" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
-      <c r="F51" t="s">
+      <c r="J51" t="s">
         <v>175</v>
       </c>
-      <c r="G51" t="s">
+      <c r="K51" s="1" t="s">
         <v>176</v>
       </c>
       <c r="L51" t="s">
         <v>177</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="O51" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N51" t="s">
+      <c r="Q51" t="s">
         <v>179</v>
       </c>
-      <c r="Q51" s="5" t="s">
+    </row>
+    <row r="52" spans="1:17">
+      <c r="J52" t="s">
         <v>180</v>
       </c>
-      <c r="S51" t="s">
+      <c r="K52" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="52" spans="1:19">
       <c r="L52" t="s">
         <v>182</v>
       </c>
-      <c r="M52" t="s">
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="D53" t="s">
         <v>183</v>
       </c>
-      <c r="N52" t="s">
+      <c r="E53" t="s">
         <v>184</v>
       </c>
-      <c r="Q52" s="5"/>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="F53" t="s">
+      <c r="J53" t="s">
         <v>185</v>
       </c>
-      <c r="G53" t="s">
+      <c r="K53" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L53" t="s">
+        <v>177</v>
+      </c>
+      <c r="O53" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="L53" t="s">
+      <c r="Q53" t="s">
         <v>187</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N53" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q53" s="5" t="s">
+    </row>
+    <row r="54" spans="1:17">
+      <c r="J54" t="s">
         <v>188</v>
       </c>
-      <c r="S53" t="s">
+      <c r="K54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="L54" t="s">
+        <v>182</v>
+      </c>
+      <c r="O54" s="5"/>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="D55" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
-      <c r="L54" t="s">
+      <c r="E55" t="s">
         <v>190</v>
       </c>
-      <c r="M54" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N54" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q54" s="5"/>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="F55" t="s">
+      <c r="J55" t="s">
         <v>191</v>
       </c>
-      <c r="G55" t="s">
+      <c r="K55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L55" t="s">
+        <v>177</v>
+      </c>
+      <c r="O55" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="L55" t="s">
+      <c r="Q55" t="s">
         <v>193</v>
       </c>
-      <c r="M55" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N55" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q55" s="5" t="s">
+    </row>
+    <row r="56" spans="1:17">
+      <c r="J56" t="s">
         <v>194</v>
       </c>
-      <c r="S55" t="s">
+      <c r="K56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="L56" t="s">
+        <v>182</v>
+      </c>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="O57" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
-      <c r="L56" t="s">
+    <row r="58" spans="1:17">
+      <c r="B58" t="s">
         <v>196</v>
       </c>
-      <c r="M56" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N56" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q56" s="5"/>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q57" t="s">
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="B58" t="s">
+      <c r="E58" t="s">
+        <v>197</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58" t="s">
         <v>198</v>
       </c>
-      <c r="C58" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="O58" t="s">
         <v>199</v>
       </c>
-      <c r="G58" t="s">
-        <v>199</v>
-      </c>
-      <c r="H58" t="s">
-        <v>20</v>
-      </c>
-      <c r="J58" t="s">
+      <c r="Q58" t="s">
         <v>200</v>
       </c>
-      <c r="Q58" t="s">
+    </row>
+    <row r="59" spans="1:17">
+      <c r="D59" t="s">
         <v>201</v>
       </c>
-      <c r="S58" t="s">
+      <c r="E59" t="s">
+        <v>201</v>
+      </c>
+      <c r="H59" t="s">
+        <v>198</v>
+      </c>
+      <c r="J59" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:19">
-      <c r="F59" t="s">
+      <c r="K59" t="s">
         <v>203</v>
-      </c>
-      <c r="G59" t="s">
-        <v>203</v>
-      </c>
-      <c r="J59" t="s">
-        <v>200</v>
       </c>
       <c r="L59" t="s">
         <v>204</v>
       </c>
-      <c r="M59" t="s">
+      <c r="O59" t="s">
         <v>205</v>
       </c>
-      <c r="N59" t="s">
+      <c r="Q59" t="s">
         <v>206</v>
       </c>
-      <c r="Q59" t="s">
+    </row>
+    <row r="60" spans="1:17">
+      <c r="J60" t="s">
         <v>207</v>
       </c>
-      <c r="S59" t="s">
+      <c r="K60" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="60" spans="1:19">
       <c r="L60" t="s">
         <v>209</v>
       </c>
-      <c r="M60" t="s">
+    </row>
+    <row r="61" spans="1:17">
+      <c r="J61" t="s">
         <v>210</v>
       </c>
-      <c r="N60" t="s">
+      <c r="K61" t="s">
+        <v>124</v>
+      </c>
+      <c r="N61" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
-      <c r="L61" t="s">
+    <row r="62" spans="1:17">
+      <c r="D62" t="s">
         <v>212</v>
       </c>
-      <c r="M61" t="s">
-        <v>126</v>
-      </c>
-      <c r="P61" t="s">
+      <c r="E62" t="s">
+        <v>212</v>
+      </c>
+      <c r="H62" t="s">
+        <v>198</v>
+      </c>
+      <c r="J62" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
-      <c r="F62" t="s">
+      <c r="K62" t="s">
+        <v>203</v>
+      </c>
+      <c r="L62" t="s">
+        <v>204</v>
+      </c>
+      <c r="O62" t="s">
         <v>214</v>
       </c>
-      <c r="G62" t="s">
-        <v>214</v>
-      </c>
-      <c r="J62" t="s">
-        <v>200</v>
-      </c>
-      <c r="L62" t="s">
+      <c r="Q62" t="s">
         <v>215</v>
       </c>
-      <c r="M62" t="s">
-        <v>205</v>
-      </c>
-      <c r="N62" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q62" t="s">
+    </row>
+    <row r="63" spans="1:17">
+      <c r="J63" t="s">
         <v>216</v>
       </c>
-      <c r="S62" t="s">
+      <c r="K63" t="s">
+        <v>124</v>
+      </c>
+      <c r="N63" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="J64" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="63" spans="1:19">
-      <c r="L63" t="s">
+      <c r="K64" t="s">
         <v>218</v>
       </c>
-      <c r="M63" t="s">
-        <v>126</v>
-      </c>
-      <c r="P63" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19">
       <c r="L64" t="s">
         <v>219</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>220</v>
       </c>
-      <c r="N64" t="s">
+    </row>
+    <row r="65" spans="1:17">
+      <c r="D65" t="s">
         <v>221</v>
       </c>
-      <c r="P64" t="s">
+      <c r="E65" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
-      <c r="F65" t="s">
+      <c r="H65" t="s">
+        <v>198</v>
+      </c>
+      <c r="J65" t="s">
         <v>223</v>
       </c>
-      <c r="G65" t="s">
+      <c r="K65" t="s">
+        <v>61</v>
+      </c>
+      <c r="L65" t="s">
+        <v>62</v>
+      </c>
+      <c r="O65" t="s">
         <v>224</v>
       </c>
-      <c r="J65" t="s">
-        <v>200</v>
-      </c>
-      <c r="L65" t="s">
+      <c r="Q65" t="s">
         <v>225</v>
       </c>
-      <c r="M65" t="s">
-        <v>63</v>
-      </c>
-      <c r="N65" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q65" t="s">
+    </row>
+    <row r="66" spans="1:17">
+      <c r="J66" t="s">
         <v>226</v>
       </c>
-      <c r="S65" t="s">
+      <c r="K66" t="s">
+        <v>124</v>
+      </c>
+      <c r="N66" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="J67" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="66" spans="1:19">
-      <c r="L66" t="s">
+      <c r="K67" t="s">
+        <v>218</v>
+      </c>
+      <c r="L67" t="s">
+        <v>219</v>
+      </c>
+      <c r="N67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="s">
+        <v>52</v>
+      </c>
+      <c r="O68" t="s">
         <v>228</v>
       </c>
-      <c r="M66" t="s">
-        <v>126</v>
-      </c>
-      <c r="P66" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19">
-      <c r="L67" t="s">
+    </row>
+    <row r="69" spans="1:17">
+      <c r="B69" t="s">
         <v>229</v>
       </c>
-      <c r="M67" t="s">
-        <v>220</v>
-      </c>
-      <c r="N67" t="s">
-        <v>221</v>
-      </c>
-      <c r="P67" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19">
-      <c r="A68" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q68" t="s">
+      <c r="D69" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
-      <c r="B69" t="s">
+      <c r="E69" t="s">
         <v>231</v>
       </c>
       <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="O69" t="s">
         <v>232</v>
       </c>
-      <c r="G69" t="s">
+    </row>
+    <row r="70" spans="1:17">
+      <c r="D70" t="s">
         <v>233</v>
       </c>
-      <c r="H69" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q69" t="s">
+      <c r="E70" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="70" spans="1:19">
-      <c r="F70" t="s">
+      <c r="J70" t="s">
         <v>235</v>
       </c>
-      <c r="G70" t="s">
+      <c r="K70" t="s">
+        <v>61</v>
+      </c>
+      <c r="L70" t="s">
+        <v>62</v>
+      </c>
+      <c r="N70" t="s">
         <v>236</v>
       </c>
-      <c r="L70" t="s">
+      <c r="O70" t="s">
         <v>237</v>
       </c>
-      <c r="M70" t="s">
-        <v>63</v>
-      </c>
-      <c r="N70" t="s">
-        <v>64</v>
-      </c>
-      <c r="P70" t="s">
+    </row>
+    <row r="71" spans="1:17">
+      <c r="D71" t="s">
         <v>238</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="E71" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
-      <c r="F71" t="s">
+      <c r="J71" t="s">
         <v>240</v>
       </c>
-      <c r="G71" t="s">
+      <c r="K71" t="s">
         <v>241</v>
       </c>
       <c r="L71" t="s">
         <v>242</v>
       </c>
-      <c r="M71" t="s">
+      <c r="N71" t="s">
         <v>243</v>
       </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>244</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>245</v>
       </c>
-      <c r="Q71" t="s">
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" t="s">
         <v>246</v>
       </c>
-      <c r="S71" t="s">
+      <c r="O72" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
-      <c r="A72" t="s">
-        <v>10</v>
-      </c>
-      <c r="K72" t="s">
+    <row r="73" spans="1:17">
+      <c r="B73" t="s">
         <v>248</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="D73" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="73" spans="1:19">
-      <c r="B73" t="s">
+      <c r="E73" t="s">
         <v>250</v>
       </c>
       <c r="F73" t="s">
+        <v>18</v>
+      </c>
+      <c r="O73" t="s">
         <v>251</v>
       </c>
-      <c r="G73" t="s">
+    </row>
+    <row r="74" spans="1:17">
+      <c r="D74" t="s">
         <v>252</v>
       </c>
-      <c r="H73" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q73" t="s">
+      <c r="E74" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="74" spans="1:19">
-      <c r="F74" t="s">
+      <c r="I74" t="s">
+        <v>246</v>
+      </c>
+      <c r="P74" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="D75" t="s">
         <v>254</v>
       </c>
-      <c r="G74" t="s">
+      <c r="E75" t="s">
         <v>255</v>
       </c>
-      <c r="K74" t="s">
-        <v>248</v>
-      </c>
-      <c r="R74" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19">
-      <c r="F75" t="s">
+      <c r="I75" t="s">
+        <v>246</v>
+      </c>
+      <c r="P75" t="s">
         <v>256</v>
       </c>
-      <c r="G75" t="s">
+    </row>
+    <row r="76" spans="1:17">
+      <c r="D76" t="s">
         <v>257</v>
       </c>
-      <c r="K75" t="s">
-        <v>248</v>
-      </c>
-      <c r="R75" t="s">
+      <c r="E76" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="76" spans="1:19">
-      <c r="F76" t="s">
+      <c r="I76" t="s">
+        <v>246</v>
+      </c>
+      <c r="J76" t="s">
         <v>259</v>
       </c>
-      <c r="G76" t="s">
+      <c r="K76" t="s">
         <v>260</v>
-      </c>
-      <c r="K76" t="s">
-        <v>248</v>
       </c>
       <c r="L76" t="s">
         <v>261</v>
       </c>
-      <c r="M76" t="s">
+      <c r="N76" t="s">
         <v>262</v>
       </c>
-      <c r="N76" t="s">
+      <c r="P76" t="s">
         <v>263</v>
       </c>
-      <c r="P76" t="s">
+      <c r="Q76" t="s">
         <v>264</v>
       </c>
-      <c r="R76" t="s">
+    </row>
+    <row r="77" spans="1:17">
+      <c r="J77" t="s">
         <v>265</v>
       </c>
-      <c r="S76" t="s">
+      <c r="K77" t="s">
+        <v>124</v>
+      </c>
+      <c r="N77" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:19">
-      <c r="L77" t="s">
+    <row r="78" spans="1:17">
+      <c r="B78" t="s">
         <v>267</v>
       </c>
-      <c r="M77" t="s">
-        <v>126</v>
-      </c>
-      <c r="P77" t="s">
+      <c r="D78" t="s">
+        <v>230</v>
+      </c>
+      <c r="E78" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="78" spans="1:19">
-      <c r="B78" t="s">
+      <c r="F78" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" t="s">
         <v>269</v>
       </c>
-      <c r="F78" t="s">
-        <v>232</v>
-      </c>
-      <c r="G78" t="s">
+      <c r="O78" t="s">
         <v>270</v>
       </c>
-      <c r="H78" t="s">
-        <v>20</v>
-      </c>
-      <c r="J78" t="s">
+    </row>
+    <row r="79" spans="1:17">
+      <c r="D79" t="s">
+        <v>238</v>
+      </c>
+      <c r="E79" t="s">
         <v>271</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="H79" t="s">
+        <v>269</v>
+      </c>
+      <c r="O79" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="79" spans="1:19">
-      <c r="F79" t="s">
-        <v>240</v>
-      </c>
-      <c r="G79" t="s">
+      <c r="Q79" t="s">
         <v>273</v>
       </c>
-      <c r="J79" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q79" t="s">
+    </row>
+    <row r="80" spans="1:17">
+      <c r="D80" t="s">
         <v>274</v>
       </c>
-      <c r="S79" t="s">
+      <c r="E80" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="80" spans="1:19">
-      <c r="F80" t="s">
+      <c r="H80" t="s">
+        <v>269</v>
+      </c>
+      <c r="O80" t="s">
         <v>276</v>
       </c>
-      <c r="G80" t="s">
+    </row>
+    <row r="81" spans="1:17">
+      <c r="D81" t="s">
         <v>277</v>
       </c>
-      <c r="J80" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q80" t="s">
+      <c r="E81" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="81" spans="1:19">
-      <c r="F81" t="s">
+      <c r="H81" t="s">
+        <v>269</v>
+      </c>
+      <c r="O81" t="s">
         <v>279</v>
       </c>
-      <c r="G81" t="s">
+    </row>
+    <row r="82" spans="1:17">
+      <c r="D82" t="s">
         <v>280</v>
       </c>
-      <c r="J81" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q81" t="s">
+      <c r="E82" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="82" spans="1:19">
-      <c r="F82" t="s">
+      <c r="J82" t="s">
         <v>282</v>
       </c>
-      <c r="G82" t="s">
+      <c r="K82" t="s">
         <v>283</v>
       </c>
-      <c r="L82" t="s">
+      <c r="M82">
+        <v>2</v>
+      </c>
+      <c r="N82" t="s">
         <v>284</v>
       </c>
-      <c r="M82" t="s">
+      <c r="O82" t="s">
         <v>285</v>
       </c>
-      <c r="O82">
-        <v>2</v>
-      </c>
-      <c r="P82" t="s">
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" t="s">
+        <v>52</v>
+      </c>
+      <c r="O83" t="s">
         <v>286</v>
       </c>
-      <c r="Q82" t="s">
+    </row>
+    <row r="84" spans="1:17">
+      <c r="B84" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="83" spans="1:19">
-      <c r="A83" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q83" t="s">
+      <c r="D84" t="s">
+        <v>230</v>
+      </c>
+      <c r="E84" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="84" spans="1:19">
-      <c r="B84" t="s">
+      <c r="F84" t="s">
+        <v>18</v>
+      </c>
+      <c r="H84" t="s">
         <v>289</v>
       </c>
-      <c r="F84" t="s">
-        <v>232</v>
-      </c>
-      <c r="G84" t="s">
+      <c r="O84" t="s">
         <v>290</v>
       </c>
-      <c r="H84" t="s">
-        <v>20</v>
-      </c>
-      <c r="J84" t="s">
+    </row>
+    <row r="85" spans="1:17">
+      <c r="D85" t="s">
         <v>291</v>
       </c>
-      <c r="Q84" t="s">
+      <c r="E85" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="85" spans="1:19">
-      <c r="F85" t="s">
+      <c r="H85" t="s">
+        <v>289</v>
+      </c>
+      <c r="O85" t="s">
         <v>293</v>
       </c>
-      <c r="G85" t="s">
+    </row>
+    <row r="86" spans="1:17">
+      <c r="D86" t="s">
         <v>294</v>
       </c>
-      <c r="J85" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q85" t="s">
+      <c r="E86" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="86" spans="1:19">
-      <c r="F86" t="s">
+      <c r="H86" t="s">
+        <v>289</v>
+      </c>
+      <c r="O86" t="s">
         <v>296</v>
       </c>
-      <c r="G86" t="s">
+    </row>
+    <row r="87" spans="1:17">
+      <c r="B87" t="s">
         <v>297</v>
       </c>
-      <c r="J86" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q86" t="s">
+      <c r="D87" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="87" spans="1:19">
-      <c r="B87" t="s">
+      <c r="E87" t="s">
         <v>299</v>
       </c>
       <c r="F87" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" t="s">
         <v>300</v>
       </c>
-      <c r="G87" t="s">
+      <c r="O87" t="s">
         <v>301</v>
       </c>
-      <c r="H87" t="s">
-        <v>20</v>
-      </c>
-      <c r="J87" t="s">
+      <c r="Q87" t="s">
         <v>302</v>
       </c>
-      <c r="Q87" t="s">
+    </row>
+    <row r="88" spans="1:17">
+      <c r="D88" t="s">
         <v>303</v>
       </c>
-      <c r="S87" t="s">
+      <c r="E88" s="6" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="88" spans="1:19">
-      <c r="F88" t="s">
+      <c r="H88" t="s">
+        <v>300</v>
+      </c>
+      <c r="O88" t="s">
         <v>305</v>
       </c>
-      <c r="G88" s="6" t="s">
+      <c r="Q88" t="s">
         <v>306</v>
       </c>
-      <c r="J88" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q88" t="s">
+    </row>
+    <row r="89" spans="1:17">
+      <c r="D89" t="s">
         <v>307</v>
       </c>
-      <c r="S88" t="s">
+      <c r="E89" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="89" spans="1:19">
-      <c r="F89" t="s">
+      <c r="H89" t="s">
+        <v>300</v>
+      </c>
+      <c r="O89" t="s">
         <v>309</v>
       </c>
-      <c r="G89" t="s">
+      <c r="Q89" t="s">
         <v>310</v>
       </c>
-      <c r="J89" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q89" t="s">
+    </row>
+    <row r="90" spans="1:17">
+      <c r="D90" t="s">
         <v>311</v>
       </c>
-      <c r="S89" t="s">
+      <c r="E90" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="90" spans="1:19">
-      <c r="F90" t="s">
+      <c r="H90" t="s">
+        <v>300</v>
+      </c>
+      <c r="O90" t="s">
         <v>313</v>
       </c>
-      <c r="G90" t="s">
+      <c r="Q90" t="s">
         <v>314</v>
       </c>
-      <c r="J90" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q90" t="s">
+    </row>
+    <row r="91" spans="1:17">
+      <c r="D91" t="s">
         <v>315</v>
       </c>
-      <c r="S90" t="s">
+      <c r="E91" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="91" spans="1:19">
-      <c r="F91" t="s">
+      <c r="H91" t="s">
+        <v>300</v>
+      </c>
+      <c r="O91" t="s">
         <v>317</v>
       </c>
-      <c r="G91" t="s">
+      <c r="Q91" t="s">
         <v>318</v>
       </c>
-      <c r="J91" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q91" t="s">
+    </row>
+    <row r="92" spans="1:17">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" t="s">
         <v>319</v>
       </c>
-      <c r="S91" t="s">
+      <c r="O92" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
-      <c r="A92" t="s">
-        <v>10</v>
-      </c>
-      <c r="K92" t="s">
+    <row r="93" spans="1:17">
+      <c r="B93" t="s">
         <v>321</v>
       </c>
-      <c r="Q92" t="s">
+      <c r="C93" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="93" spans="1:19">
-      <c r="B93" t="s">
+      <c r="E93" t="s">
         <v>323</v>
       </c>
-      <c r="C93" t="s">
-        <v>20</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="I93" t="s">
+        <v>319</v>
+      </c>
+      <c r="P93" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="D94" t="s">
         <v>324</v>
       </c>
-      <c r="G93" t="s">
+      <c r="E94" t="s">
         <v>325</v>
       </c>
-      <c r="K93" t="s">
-        <v>321</v>
-      </c>
-      <c r="R93" t="s">
+      <c r="I94" t="s">
+        <v>319</v>
+      </c>
+      <c r="P94" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
-      <c r="F94" t="s">
+    <row r="95" spans="1:17">
+      <c r="D95" t="s">
         <v>326</v>
       </c>
-      <c r="G94" t="s">
+      <c r="E95" t="s">
         <v>327</v>
       </c>
-      <c r="K94" t="s">
-        <v>321</v>
-      </c>
-      <c r="R94" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19">
-      <c r="F95" t="s">
+      <c r="I95" t="s">
+        <v>319</v>
+      </c>
+      <c r="P95" t="s">
         <v>328</v>
       </c>
-      <c r="G95" t="s">
+    </row>
+    <row r="96" spans="1:17">
+      <c r="B96" t="s">
         <v>329</v>
       </c>
-      <c r="K95" t="s">
-        <v>321</v>
-      </c>
-      <c r="R95" t="s">
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="96" spans="1:19">
-      <c r="B96" t="s">
+      <c r="E96" t="s">
         <v>331</v>
       </c>
-      <c r="C96" t="s">
-        <v>20</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="J96" t="s">
         <v>332</v>
       </c>
-      <c r="G96" t="s">
+      <c r="K96" t="s">
         <v>333</v>
       </c>
       <c r="L96" t="s">
         <v>334</v>
       </c>
-      <c r="M96" t="s">
+      <c r="O96" t="s">
         <v>335</v>
       </c>
-      <c r="N96" t="s">
+      <c r="Q96" t="s">
         <v>336</v>
       </c>
-      <c r="Q96" t="s">
+    </row>
+    <row r="97" spans="1:17">
+      <c r="J97" t="s">
         <v>337</v>
       </c>
-      <c r="S96" t="s">
+      <c r="K97" t="s">
+        <v>203</v>
+      </c>
+      <c r="L97" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17">
+      <c r="J98" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="97" spans="1:19">
-      <c r="L97" t="s">
+      <c r="K98" t="s">
         <v>339</v>
       </c>
-      <c r="M97" t="s">
-        <v>205</v>
-      </c>
-      <c r="N97" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19">
       <c r="L98" t="s">
         <v>340</v>
       </c>
-      <c r="M98" t="s">
+    </row>
+    <row r="99" spans="1:17">
+      <c r="D99" t="s">
         <v>341</v>
       </c>
-      <c r="N98" t="s">
+      <c r="E99" t="s">
+        <v>341</v>
+      </c>
+      <c r="J99" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="99" spans="1:19">
-      <c r="F99" t="s">
+      <c r="K99" t="s">
+        <v>203</v>
+      </c>
+      <c r="L99" t="s">
+        <v>204</v>
+      </c>
+      <c r="O99" t="s">
         <v>343</v>
       </c>
-      <c r="G99" t="s">
-        <v>343</v>
-      </c>
-      <c r="L99" t="s">
+      <c r="Q99" t="s">
         <v>344</v>
       </c>
-      <c r="M99" t="s">
-        <v>205</v>
-      </c>
-      <c r="N99" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q99" t="s">
+    </row>
+    <row r="100" spans="1:17">
+      <c r="J100" t="s">
         <v>345</v>
       </c>
-      <c r="S99" t="s">
+      <c r="K100" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="100" spans="1:19">
       <c r="L100" t="s">
         <v>347</v>
       </c>
-      <c r="M100" t="s">
+    </row>
+    <row r="101" spans="1:17">
+      <c r="D101" t="s">
         <v>348</v>
       </c>
-      <c r="N100" t="s">
+      <c r="E101" t="s">
+        <v>348</v>
+      </c>
+      <c r="F101" t="s">
+        <v>18</v>
+      </c>
+      <c r="H101" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="101" spans="1:19">
-      <c r="F101" t="s">
+      <c r="O101" t="s">
         <v>350</v>
       </c>
-      <c r="G101" t="s">
-        <v>350</v>
-      </c>
-      <c r="H101" t="s">
-        <v>20</v>
-      </c>
-      <c r="J101" t="s">
+      <c r="Q101" t="s">
         <v>351</v>
       </c>
-      <c r="Q101" t="s">
+    </row>
+    <row r="102" spans="1:17">
+      <c r="D102" t="s">
         <v>352</v>
       </c>
-      <c r="S101" t="s">
+      <c r="E102" t="s">
+        <v>352</v>
+      </c>
+      <c r="H102" t="s">
+        <v>349</v>
+      </c>
+      <c r="J102" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="102" spans="1:19">
-      <c r="F102" t="s">
+      <c r="K102" t="s">
+        <v>203</v>
+      </c>
+      <c r="L102" t="s">
+        <v>204</v>
+      </c>
+      <c r="O102" t="s">
         <v>354</v>
       </c>
-      <c r="G102" t="s">
-        <v>354</v>
-      </c>
-      <c r="J102" t="s">
-        <v>351</v>
-      </c>
-      <c r="L102" t="s">
+      <c r="Q102" t="s">
         <v>355</v>
       </c>
-      <c r="M102" t="s">
-        <v>205</v>
-      </c>
-      <c r="N102" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q102" t="s">
+    </row>
+    <row r="103" spans="1:17">
+      <c r="J103" t="s">
         <v>356</v>
       </c>
-      <c r="S102" t="s">
+      <c r="K103" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="103" spans="1:19">
       <c r="L103" t="s">
         <v>358</v>
       </c>
-      <c r="M103" t="s">
+    </row>
+    <row r="104" spans="1:17">
+      <c r="J104" t="s">
         <v>359</v>
       </c>
-      <c r="N103" t="s">
+      <c r="K104" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="104" spans="1:19">
       <c r="L104" t="s">
         <v>361</v>
       </c>
-      <c r="M104" t="s">
+    </row>
+    <row r="105" spans="1:17">
+      <c r="D105" t="s">
         <v>362</v>
       </c>
-      <c r="N104" t="s">
+      <c r="E105" t="s">
+        <v>362</v>
+      </c>
+      <c r="H105" t="s">
+        <v>198</v>
+      </c>
+      <c r="J105" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="105" spans="1:19">
-      <c r="F105" t="s">
+      <c r="K105" t="s">
         <v>364</v>
       </c>
-      <c r="G105" t="s">
+      <c r="N105" t="s">
+        <v>365</v>
+      </c>
+      <c r="O105" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="J106" t="s">
+        <v>368</v>
+      </c>
+      <c r="K106" t="s">
+        <v>124</v>
+      </c>
+      <c r="N106" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="J107" t="s">
+        <v>370</v>
+      </c>
+      <c r="K107" t="s">
         <v>364</v>
       </c>
-      <c r="J105" t="s">
-        <v>200</v>
-      </c>
-      <c r="L105" t="s">
-        <v>365</v>
-      </c>
-      <c r="M105" t="s">
-        <v>366</v>
-      </c>
-      <c r="P105" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>368</v>
-      </c>
-      <c r="S105" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19">
-      <c r="L106" t="s">
-        <v>370</v>
-      </c>
-      <c r="M106" t="s">
-        <v>126</v>
-      </c>
-      <c r="P106" t="s">
+      <c r="N107" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="107" spans="1:19">
-      <c r="L107" t="s">
+    <row r="108" spans="1:17">
+      <c r="J108" t="s">
         <v>372</v>
       </c>
-      <c r="M107" t="s">
-        <v>366</v>
-      </c>
-      <c r="P107" t="s">
+      <c r="K108" t="s">
+        <v>364</v>
+      </c>
+      <c r="N108" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="108" spans="1:19">
-      <c r="L108" t="s">
+    <row r="109" spans="1:17">
+      <c r="D109" t="s">
         <v>374</v>
       </c>
-      <c r="M108" t="s">
-        <v>366</v>
-      </c>
-      <c r="P108" t="s">
+      <c r="E109" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="109" spans="1:19">
-      <c r="F109" t="s">
+      <c r="H109" t="s">
+        <v>198</v>
+      </c>
+      <c r="O109" t="s">
         <v>376</v>
       </c>
-      <c r="G109" t="s">
+      <c r="Q109" t="s">
         <v>377</v>
       </c>
-      <c r="J109" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q109" t="s">
+    </row>
+    <row r="110" spans="1:17">
+      <c r="A110" t="s">
+        <v>52</v>
+      </c>
+      <c r="O110" t="s">
         <v>378</v>
       </c>
-      <c r="S109" t="s">
+    </row>
+    <row r="111" spans="1:17">
+      <c r="B111" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="110" spans="1:19">
-      <c r="A110" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q110" t="s">
+      <c r="D111" t="s">
+        <v>230</v>
+      </c>
+      <c r="E111" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="111" spans="1:19">
-      <c r="B111" t="s">
+      <c r="F111" t="s">
+        <v>18</v>
+      </c>
+      <c r="O111" t="s">
         <v>381</v>
       </c>
-      <c r="F111" t="s">
-        <v>232</v>
-      </c>
-      <c r="G111" t="s">
+    </row>
+    <row r="112" spans="1:17">
+      <c r="D112" t="s">
         <v>382</v>
       </c>
-      <c r="H111" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q111" t="s">
+      <c r="E112" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="112" spans="1:19">
-      <c r="F112" t="s">
+      <c r="O112" t="s">
         <v>384</v>
       </c>
-      <c r="G112" t="s">
+    </row>
+    <row r="113" spans="1:17">
+      <c r="D113" t="s">
         <v>385</v>
       </c>
-      <c r="Q112" t="s">
+      <c r="E113" t="s">
+        <v>385</v>
+      </c>
+      <c r="O113" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="113" spans="1:19">
-      <c r="F113" t="s">
+      <c r="Q113" t="s">
         <v>387</v>
       </c>
-      <c r="G113" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q113" t="s">
+    </row>
+    <row r="114" spans="1:17">
+      <c r="D114" t="s">
         <v>388</v>
       </c>
-      <c r="S113" t="s">
+      <c r="E114" t="s">
+        <v>388</v>
+      </c>
+      <c r="J114" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="114" spans="1:19">
-      <c r="F114" t="s">
+      <c r="K114" t="s">
+        <v>203</v>
+      </c>
+      <c r="L114" t="s">
+        <v>204</v>
+      </c>
+      <c r="N114" t="s">
         <v>390</v>
       </c>
-      <c r="G114" t="s">
-        <v>390</v>
-      </c>
-      <c r="L114" t="s">
+      <c r="O114" t="s">
         <v>391</v>
       </c>
-      <c r="M114" t="s">
-        <v>205</v>
-      </c>
-      <c r="N114" t="s">
-        <v>206</v>
-      </c>
-      <c r="P114" t="s">
+      <c r="Q114" t="s">
         <v>392</v>
       </c>
-      <c r="Q114" t="s">
+    </row>
+    <row r="115" spans="1:17">
+      <c r="A115" t="s">
+        <v>52</v>
+      </c>
+      <c r="O115" t="s">
         <v>393</v>
       </c>
-      <c r="S114" t="s">
+    </row>
+    <row r="116" spans="1:17">
+      <c r="B116" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="115" spans="1:19">
-      <c r="A115" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q115" t="s">
+      <c r="D116" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="116" spans="1:19">
-      <c r="B116" t="s">
+      <c r="E116" t="s">
         <v>396</v>
       </c>
       <c r="F116" t="s">
+        <v>18</v>
+      </c>
+      <c r="O116" t="s">
         <v>397</v>
       </c>
-      <c r="G116" t="s">
+    </row>
+    <row r="117" spans="1:17">
+      <c r="D117" t="s">
         <v>398</v>
       </c>
-      <c r="H116" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q116" t="s">
+      <c r="E117" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="117" spans="1:19">
-      <c r="F117" t="s">
+      <c r="J117" t="s">
         <v>400</v>
       </c>
-      <c r="G117" t="s">
+      <c r="K117" t="s">
+        <v>203</v>
+      </c>
+      <c r="L117" t="s">
+        <v>204</v>
+      </c>
+      <c r="O117" t="s">
         <v>401</v>
       </c>
-      <c r="L117" t="s">
+      <c r="Q117" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17">
+      <c r="J118" t="s">
         <v>402</v>
       </c>
-      <c r="M117" t="s">
-        <v>205</v>
-      </c>
-      <c r="N117" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q117" t="s">
+      <c r="K118" t="s">
         <v>403</v>
       </c>
-      <c r="S117" t="s">
+      <c r="L118" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
+      <c r="J119" t="s">
+        <v>404</v>
+      </c>
+      <c r="K119" t="s">
+        <v>181</v>
+      </c>
+      <c r="L119" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
+      <c r="D120" t="s">
+        <v>405</v>
+      </c>
+      <c r="E120" t="s">
+        <v>406</v>
+      </c>
+      <c r="J120" t="s">
+        <v>407</v>
+      </c>
+      <c r="K120" t="s">
+        <v>61</v>
+      </c>
+      <c r="L120" t="s">
+        <v>62</v>
+      </c>
+      <c r="O120" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17">
+      <c r="J121" t="s">
+        <v>409</v>
+      </c>
+      <c r="K121" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="118" spans="1:19">
-      <c r="L118" t="s">
-        <v>404</v>
-      </c>
-      <c r="M118" t="s">
-        <v>405</v>
-      </c>
-      <c r="N118" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19">
-      <c r="L119" t="s">
-        <v>406</v>
-      </c>
-      <c r="M119" t="s">
-        <v>183</v>
-      </c>
-      <c r="N119" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19">
-      <c r="F120" t="s">
-        <v>407</v>
-      </c>
-      <c r="G120" t="s">
-        <v>408</v>
-      </c>
-      <c r="L120" t="s">
-        <v>409</v>
-      </c>
-      <c r="M120" t="s">
-        <v>63</v>
-      </c>
-      <c r="N120" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q120" t="s">
+      <c r="L121" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
+      <c r="J122" t="s">
         <v>410</v>
       </c>
-      <c r="S120" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19">
-      <c r="L121" t="s">
+      <c r="K122" t="s">
+        <v>181</v>
+      </c>
+      <c r="L122" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
+      <c r="A123" t="s">
+        <v>52</v>
+      </c>
+      <c r="O123" t="s">
         <v>411</v>
       </c>
-      <c r="M121" t="s">
-        <v>405</v>
-      </c>
-      <c r="N121" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19">
-      <c r="L122" t="s">
+    </row>
+    <row r="124" spans="1:17">
+      <c r="A124" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" t="s">
         <v>412</v>
       </c>
-      <c r="M122" t="s">
-        <v>183</v>
-      </c>
-      <c r="N122" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19">
-      <c r="A123" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q123" t="s">
+      <c r="O124" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="124" spans="1:19">
-      <c r="A124" t="s">
-        <v>10</v>
-      </c>
-      <c r="K124" t="s">
+    <row r="125" spans="1:17">
+      <c r="B125" t="s">
         <v>414</v>
       </c>
-      <c r="Q124" t="s">
+      <c r="C125" t="s">
+        <v>18</v>
+      </c>
+      <c r="D125" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="125" spans="1:19">
-      <c r="B125" t="s">
+      <c r="E125" t="s">
         <v>416</v>
       </c>
-      <c r="C125" t="s">
-        <v>20</v>
-      </c>
       <c r="F125" t="s">
+        <v>18</v>
+      </c>
+      <c r="O125" t="s">
         <v>417</v>
       </c>
-      <c r="G125" t="s">
+    </row>
+    <row r="126" spans="1:17">
+      <c r="D126" t="s">
         <v>418</v>
       </c>
-      <c r="H125" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q125" t="s">
+      <c r="E126" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="126" spans="1:19">
-      <c r="F126" t="s">
+      <c r="I126" t="s">
+        <v>412</v>
+      </c>
+      <c r="J126" t="s">
         <v>420</v>
       </c>
-      <c r="G126" t="s">
+      <c r="K126" t="s">
+        <v>218</v>
+      </c>
+      <c r="L126" t="s">
+        <v>219</v>
+      </c>
+      <c r="P126" t="s">
         <v>421</v>
       </c>
-      <c r="K126" t="s">
-        <v>414</v>
-      </c>
-      <c r="L126" t="s">
+    </row>
+    <row r="127" spans="1:17">
+      <c r="D127" t="s">
         <v>422</v>
       </c>
-      <c r="M126" t="s">
-        <v>220</v>
-      </c>
-      <c r="N126" t="s">
-        <v>221</v>
-      </c>
-      <c r="R126" t="s">
+      <c r="E127" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="127" spans="1:19">
-      <c r="F127" t="s">
+      <c r="I127" t="s">
+        <v>412</v>
+      </c>
+      <c r="J127" t="s">
         <v>424</v>
       </c>
-      <c r="G127" t="s">
+      <c r="K127" t="s">
+        <v>203</v>
+      </c>
+      <c r="L127" t="s">
+        <v>204</v>
+      </c>
+      <c r="P127" t="s">
         <v>425</v>
       </c>
-      <c r="K127" t="s">
-        <v>414</v>
-      </c>
-      <c r="L127" t="s">
+    </row>
+    <row r="128" spans="1:17">
+      <c r="J128" t="s">
         <v>426</v>
       </c>
-      <c r="M127" t="s">
-        <v>205</v>
-      </c>
-      <c r="N127" t="s">
-        <v>206</v>
-      </c>
-      <c r="R127" t="s">
+      <c r="K128" t="s">
+        <v>218</v>
+      </c>
+      <c r="L128" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="129" spans="4:17">
+      <c r="D129" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="128" spans="1:19">
-      <c r="L128" t="s">
+      <c r="E129" t="s">
+        <v>427</v>
+      </c>
+      <c r="I129" t="s">
+        <v>412</v>
+      </c>
+      <c r="J129" t="s">
         <v>428</v>
       </c>
-      <c r="M128" t="s">
-        <v>220</v>
-      </c>
-      <c r="N128" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="129" spans="6:19">
-      <c r="F129" t="s">
+      <c r="K129" t="s">
+        <v>203</v>
+      </c>
+      <c r="L129" t="s">
+        <v>204</v>
+      </c>
+      <c r="P129" t="s">
         <v>429</v>
       </c>
-      <c r="G129" t="s">
-        <v>429</v>
-      </c>
-      <c r="K129" t="s">
-        <v>414</v>
-      </c>
-      <c r="L129" t="s">
+    </row>
+    <row r="130" spans="4:17">
+      <c r="J130" t="s">
         <v>430</v>
       </c>
-      <c r="M129" t="s">
-        <v>205</v>
-      </c>
-      <c r="N129" t="s">
-        <v>206</v>
-      </c>
-      <c r="R129" t="s">
+      <c r="K130" t="s">
+        <v>218</v>
+      </c>
+      <c r="L130" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="131" spans="4:17">
+      <c r="D131" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="130" spans="6:19">
-      <c r="L130" t="s">
+      <c r="E131" t="s">
+        <v>431</v>
+      </c>
+      <c r="J131" t="s">
         <v>432</v>
       </c>
-      <c r="M130" t="s">
-        <v>220</v>
-      </c>
-      <c r="N130" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="131" spans="6:19">
-      <c r="F131" t="s">
-        <v>433</v>
-      </c>
-      <c r="G131" t="s">
+      <c r="K131" t="s">
         <v>433</v>
       </c>
       <c r="L131" t="s">
         <v>434</v>
       </c>
-      <c r="M131" t="s">
+      <c r="N131" t="s">
         <v>435</v>
       </c>
-      <c r="N131" t="s">
+      <c r="O131" t="s">
         <v>436</v>
       </c>
-      <c r="P131" t="s">
+      <c r="Q131" t="s">
         <v>437</v>
       </c>
-      <c r="Q131" t="s">
+    </row>
+    <row r="132" spans="4:17">
+      <c r="J132" t="s">
         <v>438</v>
       </c>
-      <c r="S131" t="s">
+      <c r="K132" t="s">
+        <v>364</v>
+      </c>
+      <c r="N132" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="132" spans="6:19">
-      <c r="L132" t="s">
-        <v>440</v>
-      </c>
-      <c r="M132" t="s">
-        <v>366</v>
-      </c>
-      <c r="P132" t="s">
-        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>